<commit_message>
Überarbeitung /Anpassung Evaluation View
</commit_message>
<xml_diff>
--- a/BWB-Auswertung/Resources/Vorlagen/Gruppendaten.xlsx
+++ b/BWB-Auswertung/Resources/Vorlagen/Gruppendaten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\jf-bundeswettbewerb\BWB-Auswertung\BWB-Auswertung\Resources\Vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\BWB-Auswertung\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DC9A292-C28F-46EF-9D66-94B2C12E410B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C579F-B68A-47F9-A71C-0306582C4F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
+    <workbookView xWindow="51615" yWindow="3600" windowWidth="38700" windowHeight="15345" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -44,18 +44,6 @@
     <t>Feuerwehr</t>
   </si>
   <si>
-    <t>Gruppe</t>
-  </si>
-  <si>
-    <t>StartNR</t>
-  </si>
-  <si>
-    <t>Platz</t>
-  </si>
-  <si>
-    <t>Gesamtpunkte</t>
-  </si>
-  <si>
     <t>Geschlecht</t>
   </si>
   <si>
@@ -72,6 +60,18 @@
   </si>
   <si>
     <t>Geburtsdatum</t>
+  </si>
+  <si>
+    <t>LagerNr</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Essgewohnheiten</t>
+  </si>
+  <si>
+    <t>Unverträglichkeiten</t>
   </si>
 </sst>
 </file>
@@ -144,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -290,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -443,30 +443,29 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:11" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,31 +473,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes Import und Darstellung von Gruppen
</commit_message>
<xml_diff>
--- a/BWB-Auswertung/Resources/Vorlagen/Gruppendaten.xlsx
+++ b/BWB-Auswertung/Resources/Vorlagen/Gruppendaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\kzl-teilnehmenden-auswertung\BWB-Auswertung\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C579F-B68A-47F9-A71C-0306582C4F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F074A05D-AF8F-4C26-9098-B92238F38DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51615" yWindow="3600" windowWidth="38700" windowHeight="15345" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="38700" windowHeight="15345" xr2:uid="{46DC5956-F28C-4B63-B268-66BCF5D1ECC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>